<commit_message>
Mise à jour 0.1.1a - Correction de bug de merging
Correction de bug de merging qu'il y a eu dans le fichier
"EcranChangementPerso.xaml.cs" entre Tommy et moi-même.
</commit_message>
<xml_diff>
--- a/BUG TRACKER.xlsx
+++ b/BUG TRACKER.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>NUM</t>
   </si>
@@ -48,7 +48,25 @@
     <t>Profession.cs et professionService.cs et creationPersonnage.xaml.cs</t>
   </si>
   <si>
-    <t xml:space="preserve">à corrigé </t>
+    <t xml:space="preserve">Corrigé par Anthony </t>
+  </si>
+  <si>
+    <t>23/10/2014 - 23h24</t>
+  </si>
+  <si>
+    <t>Erreur d'affichage des points de vie/énergie dans choix du personnage</t>
+  </si>
+  <si>
+    <t>L'affichage est toujours "19" Peut importe ce qu'on passe… Pourtant, quand on regarde dans le debug on essaie bien de mettre "Énergie: x"</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>EcranChangementPerso.xaml.cs</t>
+  </si>
+  <si>
+    <t>23/10/2014 - 23h33</t>
   </si>
 </sst>
 </file>
@@ -108,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -120,11 +138,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,7 +171,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -426,13 +457,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
     <col min="3" max="3" width="52.5703125" customWidth="1"/>
@@ -441,7 +472,7 @@
     <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -477,235 +508,558 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="F16" s="7"/>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="F17" s="7"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="F18" s="7"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="F19" s="7"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="F21" s="7"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="F22" s="7"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
     </row>
   </sheetData>
@@ -720,7 +1074,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -732,7 +1086,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>